<commit_message>
updated filename references and uploaded templates to ligand mpnn
</commit_message>
<xml_diff>
--- a/mes-binder/eosin-y/eos_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/eosin-y/eos_ligand_mpnn_filename_ref.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\mes-binder\eosin-y\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\enzyme_engineering\mes-binder\eosin-y\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{325F136A-FBEA-4638-B95A-4B19071AC0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95CBBD2-C409-4677-9713-3AF56F0EB175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="135" windowWidth="15300" windowHeight="7785" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="for ligand MPNN" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Original protein</t>
   </si>
@@ -54,13 +54,37 @@
     <t>EOS</t>
   </si>
   <si>
-    <t>7au_eos_5A</t>
-  </si>
-  <si>
     <t>residues within 5A</t>
   </si>
   <si>
     <t>7au_eos_5A-2</t>
+  </si>
+  <si>
+    <t>residues within 8A</t>
+  </si>
+  <si>
+    <t>7au_eos_5A-1</t>
+  </si>
+  <si>
+    <t>7au_eos_8A-1</t>
+  </si>
+  <si>
+    <t>7au_eos_8A-2</t>
+  </si>
+  <si>
+    <t>7au_eos_8A-3</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>7au_eos_mpnn-1</t>
+  </si>
+  <si>
+    <t>7au_eos_mpnn-2</t>
+  </si>
+  <si>
+    <t>protein mpnn entire</t>
   </si>
 </sst>
 </file>
@@ -83,12 +107,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,10 +133,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9FB470-8A86-4005-97EB-66EB0B37B6A1}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,22 +506,18 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>45446</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3">
         <v>4</v>
       </c>
@@ -498,18 +525,107 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1">
         <v>45446</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="1">
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1">
         <v>45446</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docking for most of 7auy-eosin structures done
</commit_message>
<xml_diff>
--- a/mes-binder/eosin-y/eos_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/eosin-y/eos_ligand_mpnn_filename_ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\mes-binder\eosin-y\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2508821-35B7-4ED3-9237-742D754C4E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CFD0C3-A058-4608-84B1-C34650573AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-540" yWindow="2430" windowWidth="18090" windowHeight="17130" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="13110" yWindow="2700" windowWidth="26205" windowHeight="17130" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="diffusion -&gt; protein mpnn -&gt; AF" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t>Original protein</t>
   </si>
@@ -182,6 +182,58 @@
   </si>
   <si>
     <t>7au_eos_mpnn-2_lig_3</t>
+  </si>
+  <si>
+    <t>Docking affinity (best model autodock vina)</t>
+  </si>
+  <si>
+    <t>Rejected, steric clash</t>
+  </si>
+  <si>
+    <t>Rejected, steric clash (-8.165)</t>
+  </si>
+  <si>
+    <t>Rejected, steric clash, (-7.912)</t>
+  </si>
+  <si>
+    <t>Rejected, steric clash (-7.415)</t>
+  </si>
+  <si>
+    <t>steric clash, -7.576</t>
+  </si>
+  <si>
+    <t>some clash, -7.695</t>
+  </si>
+  <si>
+    <t>slight clash, -8.268</t>
+  </si>
+  <si>
+    <t>slight clash, -7.458</t>
+  </si>
+  <si>
+    <t>rejected, steric clash ( -8.707)</t>
+  </si>
+  <si>
+    <t>Note: If the affinity is just "rejected, steric clash" it means when ligand mpnn structure is aligned to the original diffused template, obvious steric clash was visible. If there is an affinity value in brackets, it means docking was performed but there was steric clash so it was rejected after docking.
+For those in black font, it means there is some clash after docking but has potential:
+steric clash - dockx clash values &gt;= 300
+some clash - dockx clash values &gt;=150
+slight clash - dockx clash values &lt; 150</t>
+  </si>
+  <si>
+    <t>some clash, -8.477</t>
+  </si>
+  <si>
+    <t>slight clash, -8.298</t>
+  </si>
+  <si>
+    <t>slight clash, -7.349, chosen</t>
+  </si>
+  <si>
+    <t>rejected, steric clash (-8.237)</t>
+  </si>
+  <si>
+    <t>-7.804 (best so far)</t>
   </si>
 </sst>
 </file>
@@ -236,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -249,6 +301,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -567,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9FB470-8A86-4005-97EB-66EB0B37B6A1}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,10 +890,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E6AFCC-98DF-46AC-8D4A-879C6C06E4E0}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,9 +905,10 @@
     <col min="5" max="5" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="40.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -865,8 +933,14 @@
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -891,8 +965,24 @@
       <c r="H2" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>29</v>
@@ -915,8 +1005,22 @@
       <c r="H3" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>31</v>
@@ -939,8 +1043,22 @@
       <c r="H4" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -965,8 +1083,22 @@
       <c r="H5" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>29</v>
@@ -989,8 +1121,22 @@
       <c r="H6" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>31</v>
@@ -1013,8 +1159,22 @@
       <c r="H7" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1039,8 +1199,22 @@
       <c r="H8" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>29</v>
@@ -1063,8 +1237,22 @@
       <c r="H9" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>31</v>
@@ -1087,8 +1275,22 @@
       <c r="H10" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
@@ -1113,8 +1315,22 @@
       <c r="H11" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" t="s">
         <v>29</v>
@@ -1137,8 +1353,22 @@
       <c r="H12" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" t="s">
         <v>31</v>
@@ -1161,8 +1391,22 @@
       <c r="H13" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
@@ -1187,8 +1431,22 @@
       <c r="H14" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>29</v>
@@ -1211,8 +1469,22 @@
       <c r="H15" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>31</v>
@@ -1235,9 +1507,23 @@
       <c r="H16" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="I16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
@@ -1261,9 +1547,23 @@
       <c r="H17" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="I17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1285,9 +1585,23 @@
       <c r="H18" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="I18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -1309,9 +1623,23 @@
       <c r="H19" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="I19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="1">
+        <v>45449</v>
+      </c>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1335,9 +1663,17 @@
       <c r="H20" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1359,9 +1695,17 @@
       <c r="H21" s="1">
         <v>45448</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
       <c r="B22" t="s">
         <v>31</v>
       </c>
@@ -1383,9 +1727,38 @@
       <c r="H22" s="1">
         <v>45448</v>
       </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="M2:T12"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A2:A4"/>

</xml_diff>

<commit_message>
bindings for ligand mpnn bias designs
</commit_message>
<xml_diff>
--- a/mes-binder/eosin-y/eos_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/eosin-y/eos_ligand_mpnn_filename_ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\mes-binder\eosin-y\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166FD17C-450A-4515-BEA5-601A09F2C0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDD9A1-3B71-42DE-A3C5-E3C6BE6572F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="2685" windowWidth="26205" windowHeight="17130" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="1440" yWindow="2520" windowWidth="26205" windowHeight="17130" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="diffusion -&gt; protein mpnn -&gt; AF" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,6 +323,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -332,8 +335,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,7 +661,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D8" sqref="D8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +919,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A23" sqref="A23:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +967,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
@@ -994,19 +997,19 @@
       <c r="J2" s="1">
         <v>45449</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -1034,17 +1037,17 @@
       <c r="J3" s="1">
         <v>45449</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1072,17 +1075,17 @@
       <c r="J4" s="1">
         <v>45449</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -1112,17 +1115,17 @@
       <c r="J5" s="1">
         <v>45449</v>
       </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -1150,17 +1153,17 @@
       <c r="J6" s="1">
         <v>45449</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>31</v>
       </c>
@@ -1188,17 +1191,17 @@
       <c r="J7" s="1">
         <v>45449</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
@@ -1228,17 +1231,17 @@
       <c r="J8" s="1">
         <v>45449</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>29</v>
       </c>
@@ -1266,17 +1269,17 @@
       <c r="J9" s="1">
         <v>45449</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -1304,17 +1307,17 @@
       <c r="J10" s="1">
         <v>45449</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
@@ -1344,17 +1347,17 @@
       <c r="J11" s="1">
         <v>45449</v>
       </c>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>29</v>
       </c>
@@ -1382,17 +1385,17 @@
       <c r="J12" s="1">
         <v>45449</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1430,7 +1433,7 @@
       <c r="T13" s="8"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
@@ -1470,7 +1473,7 @@
       <c r="T14" s="8"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1511,7 @@
       <c r="T15" s="8"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -1546,7 +1549,7 @@
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
@@ -1586,7 +1589,7 @@
       <c r="T17" s="8"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1624,7 +1627,7 @@
       <c r="T18" s="8"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -1646,7 +1649,7 @@
       <c r="H19" s="1">
         <v>45448</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="9" t="s">
         <v>67</v>
       </c>
       <c r="J19" s="1">
@@ -1662,7 +1665,7 @@
       <c r="T19" s="8"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1702,7 +1705,7 @@
       <c r="T20" s="8"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1740,7 +1743,7 @@
       <c r="T21" s="8"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>31</v>
       </c>
@@ -1762,7 +1765,7 @@
       <c r="H22" s="1">
         <v>45448</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="9" t="s">
         <v>70</v>
       </c>
       <c r="J22" s="1">
@@ -1778,6 +1781,7 @@
       <c r="T22" s="8"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -1788,6 +1792,7 @@
       <c r="T23" s="8"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>

</xml_diff>